<commit_message>
updating for training 0.2.3 1.6.1
</commit_message>
<xml_diff>
--- a/projects/training_NSGA1.xlsx
+++ b/projects/training_NSGA1.xlsx
@@ -2077,10 +2077,10 @@
     <t>Office NSGA</t>
   </si>
   <si>
-    <t>0.2.2</t>
-  </si>
-  <si>
-    <t>1.6.1-rc1</t>
+    <t>0.2.3</t>
+  </si>
+  <si>
+    <t>1.6.1</t>
   </si>
 </sst>
 </file>

</xml_diff>